<commit_message>
add assessment and visualization in k-means clustering
</commit_message>
<xml_diff>
--- a/clustering/clustering_results.xlsx
+++ b/clustering/clustering_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kerberos233\IdeaProjects\ATTCK_analyze module\clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92257536-76ED-4556-83D8-20ECAAC76F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC697FAE-531C-4307-987F-4DD0290BAF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>clustering algorithm type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,13 +45,23 @@
   </si>
   <si>
     <t>db_score</t>
+  </si>
+  <si>
+    <t>Agglomerative Clustering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">threshold </t>
+  </si>
+  <si>
+    <t>Agglomerative Clustering</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +79,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF374151"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF343541"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -93,9 +109,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,176 +394,344 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" customWidth="1"/>
+    <col min="2" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
         <v>0.24012821042834401</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
         <v>2.6495988086581601</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
         <v>0.14970048656774099</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <v>3.3043917481181899</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
         <v>0.14828082692851499</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
         <v>3.0172366290866002</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
         <v>0.17959533513763201</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
         <v>1.93161806735845</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
         <v>0.229029801628721</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
         <v>1.8877489953663</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>7</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
         <v>0.15468631049468301</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
         <v>2.00188297583709</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>8</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
         <v>0.17493638941089401</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
         <v>1.7614909581275799</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>9</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
         <v>4.6639536049424002E-2</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
         <v>2.0148512241051</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1.5765558228153599E-2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.123091490979332</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.32871999547509201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2.6303119323966E-2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.123091490979332</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.39648429221521198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.76210759164162E-2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.123091490979332</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.451215607200531</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3.1225335102762201E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.123091490979332</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.47743989401499398</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1">
+        <v>4.1324599268855497E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.123091490979332</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.49192457749243101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>8.5092697239507201E-2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.123091490979332</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.528080829779628</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.115731923494064</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.123091490979332</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.527708365025646</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add phi and jacarrd distance as measurement and clustering
</commit_message>
<xml_diff>
--- a/clustering/clustering_results.xlsx
+++ b/clustering/clustering_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kerberos233\IdeaProjects\ATTCK_analyze module\clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F3BD7B-6B06-43C9-AA33-A89A7060AF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10E95EF-7F93-4730-8661-A0F8F0A09FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -715,142 +715,142 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
       </c>
       <c r="D10">
-        <v>1.5765558228153599E-2</v>
+        <v>1.4410544261247501E-3</v>
       </c>
       <c r="E10">
         <v>0.123091490979332</v>
       </c>
       <c r="F10">
-        <v>0.32871999547509201</v>
+        <v>0.42506514881971502</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
       </c>
       <c r="D11">
-        <v>2.6303119323966E-2</v>
+        <v>1.60257758873238E-2</v>
       </c>
       <c r="E11">
         <v>0.123091490979332</v>
       </c>
       <c r="F11">
-        <v>0.39648429221521198</v>
+        <v>0.44371725808736501</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
       </c>
       <c r="D12">
-        <v>1.76210759164162E-2</v>
+        <v>3.05242946396635E-2</v>
       </c>
       <c r="E12">
         <v>0.123091490979332</v>
       </c>
       <c r="F12">
-        <v>0.451215607200531</v>
+        <v>0.47619916122609801</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
       </c>
       <c r="D13">
-        <v>3.1225335102762201E-2</v>
+        <v>6.2235238473548303E-2</v>
       </c>
       <c r="E13">
         <v>0.123091490979332</v>
       </c>
       <c r="F13">
-        <v>0.47743989401499398</v>
+        <v>0.479465322499672</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
       </c>
       <c r="D14">
-        <v>4.1324599268855497E-2</v>
+        <v>9.9935828479864902E-2</v>
       </c>
       <c r="E14">
         <v>0.123091490979332</v>
       </c>
       <c r="F14">
-        <v>0.49192457749243101</v>
+        <v>0.47423810904276698</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
       </c>
       <c r="D15">
-        <v>8.5092697239507201E-2</v>
+        <v>0.123793484125835</v>
       </c>
       <c r="E15">
         <v>0.123091490979332</v>
       </c>
       <c r="F15">
-        <v>0.528080829779628</v>
+        <v>0.47332401547963598</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
       </c>
       <c r="D16">
-        <v>0.115731923494064</v>
+        <v>0.17482965331112699</v>
       </c>
       <c r="E16">
         <v>0.123091490979332</v>
       </c>
       <c r="F16">
-        <v>0.527708365025646</v>
+        <v>0.47401163406782598</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -858,19 +858,19 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
         <v>28</v>
       </c>
       <c r="D17">
-        <v>1.4410544261247501E-3</v>
+        <v>0.19555361735287399</v>
       </c>
       <c r="E17">
         <v>0.123091490979332</v>
       </c>
       <c r="F17">
-        <v>0.42506514881971502</v>
+        <v>0.48027927654226898</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -878,19 +878,19 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>28</v>
       </c>
       <c r="D18">
-        <v>1.60257758873238E-2</v>
+        <v>0.214297939076114</v>
       </c>
       <c r="E18">
         <v>0.123091490979332</v>
       </c>
       <c r="F18">
-        <v>0.44371725808736501</v>
+        <v>0.48791121496020001</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -898,219 +898,219 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
         <v>28</v>
       </c>
       <c r="D19">
-        <v>3.05242946396635E-2</v>
+        <v>0.25066976726873802</v>
       </c>
       <c r="E19">
         <v>0.123091490979332</v>
       </c>
       <c r="F19">
-        <v>0.47619916122609801</v>
+        <v>0.494225090260133</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D20">
-        <v>6.2235238473548303E-2</v>
+        <v>0.29222690621332098</v>
       </c>
       <c r="E20">
         <v>0.123091490979332</v>
       </c>
       <c r="F20">
-        <v>0.479465322499672</v>
+        <v>0.47834483184524801</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>9.9935828479864902E-2</v>
+        <v>0.215708254946779</v>
       </c>
       <c r="E21">
-        <v>0.123091490979332</v>
+        <v>4.5504345235961703E-2</v>
       </c>
       <c r="F21">
-        <v>0.47423810904276698</v>
+        <v>0.62774204896770902</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>0.123793484125835</v>
+        <v>0.215708254946779</v>
       </c>
       <c r="E22">
-        <v>0.123091490979332</v>
+        <v>4.5504345235961703E-2</v>
       </c>
       <c r="F22">
-        <v>0.47332401547963598</v>
+        <v>0.62774204896770902</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>0.17482965331112699</v>
+        <v>2.6303119323966E-2</v>
       </c>
       <c r="E23">
         <v>0.123091490979332</v>
       </c>
       <c r="F23">
-        <v>0.47401163406782598</v>
+        <v>0.39648429221521198</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>0.19555361735287399</v>
+        <v>1.76210759164162E-2</v>
       </c>
       <c r="E24">
         <v>0.123091490979332</v>
       </c>
       <c r="F24">
-        <v>0.48027927654226898</v>
+        <v>0.451215607200531</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" t="s">
-        <v>28</v>
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>0.214297939076114</v>
+        <v>3.1225335102762201E-2</v>
       </c>
       <c r="E25">
         <v>0.123091490979332</v>
       </c>
       <c r="F25">
-        <v>0.48791121496020001</v>
+        <v>0.47743989401499398</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>0.25066976726873802</v>
+        <v>4.1324599268855497E-2</v>
       </c>
       <c r="E26">
         <v>0.123091490979332</v>
       </c>
       <c r="F26">
-        <v>0.494225090260133</v>
+        <v>0.49192457749243101</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>0.29222690621332098</v>
+        <v>8.5092697239507201E-2</v>
       </c>
       <c r="E27">
         <v>0.123091490979332</v>
       </c>
       <c r="F27">
-        <v>0.47834483184524801</v>
+        <v>0.528080829779628</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>0.215708254946779</v>
+        <v>0.115731923494064</v>
       </c>
       <c r="E28">
-        <v>4.5504345235961703E-2</v>
+        <v>0.123091490979332</v>
       </c>
       <c r="F28">
-        <v>0.62774204896770902</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0.215708254946779</v>
-      </c>
-      <c r="E29">
-        <v>4.5504345235961703E-2</v>
-      </c>
-      <c r="F29">
-        <v>0.62774204896770902</v>
+        <v>0.527708365025646</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>1.5765558228153599E-2</v>
+      </c>
+      <c r="E30">
+        <v>0.123091490979332</v>
+      </c>
+      <c r="F30">
+        <v>0.32871999547509201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>